<commit_message>
other end of DHCP ports
</commit_message>
<xml_diff>
--- a/06BM port info.xlsx
+++ b/06BM port info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="269">
   <si>
     <t xml:space="preserve">Switch</t>
   </si>
@@ -814,7 +814,19 @@
     <t xml:space="preserve">Look up MAC address</t>
   </si>
   <si>
+    <t xml:space="preserve">pylon 2.2</t>
+  </si>
+  <si>
     <t xml:space="preserve">DHCP port</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pylon 1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">upstream 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">downstream 6</t>
   </si>
 </sst>
 </file>
@@ -961,16 +973,16 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I153" activeCellId="0" sqref="I153:I157"/>
+      <selection pane="bottomLeft" activeCell="I156" activeCellId="0" sqref="I156"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24"/>
   </cols>
   <sheetData>
@@ -5719,9 +5731,11 @@
       <c r="H154" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I154" s="3"/>
+      <c r="I154" s="3" t="s">
+        <v>264</v>
+      </c>
       <c r="J154" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5749,9 +5763,11 @@
       <c r="H155" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I155" s="3"/>
+      <c r="I155" s="3" t="s">
+        <v>266</v>
+      </c>
       <c r="J155" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5779,9 +5795,11 @@
       <c r="H156" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I156" s="3"/>
+      <c r="I156" s="3" t="s">
+        <v>267</v>
+      </c>
       <c r="J156" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5809,9 +5827,11 @@
       <c r="H157" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I157" s="3"/>
+      <c r="I157" s="3" t="s">
+        <v>268</v>
+      </c>
       <c r="J157" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>